<commit_message>
Update of the dashboard including LBBG and LBWN
</commit_message>
<xml_diff>
--- a/data/APT_BBOX.xlsx
+++ b/data/APT_BBOX.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdlange\repos\pru-apt-dashboards\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speeters\repos\airport-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFD804C-E902-49D6-8BCD-C25B50F39997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="6" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="709">
   <si>
     <t>AIRPORT</t>
   </si>
@@ -2140,12 +2141,30 @@
   </si>
   <si>
     <t>19.23861751012485,42.343837053533804,19.257075937674294,42.375038728663945</t>
+  </si>
+  <si>
+    <t>27.471485,42.549919,27.554054,42.589362</t>
+  </si>
+  <si>
+    <t>LBBG</t>
+  </si>
+  <si>
+    <t>Burgas</t>
+  </si>
+  <si>
+    <t>LBWN</t>
+  </si>
+  <si>
+    <t>27.800088,43.226131,27.846866,43.240982</t>
+  </si>
+  <si>
+    <t>Varna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2201,7 +2220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2239,12 +2258,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2282,6 +2312,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2562,12 +2596,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,17 +2655,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>432</v>
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2639,13 +2673,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2653,13 +2687,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>212</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>435</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2667,13 +2701,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2681,13 +2715,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2695,13 +2729,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2709,13 +2743,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2723,13 +2757,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,13 +2771,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2751,13 +2785,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2765,13 +2799,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2779,13 +2813,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2793,13 +2827,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>431</v>
+        <v>28</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2807,13 +2841,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2821,83 +2855,83 @@
         <v>7</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>440</v>
+        <v>32</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>450</v>
+      <c r="B23" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2905,13 +2939,13 @@
         <v>44</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,13 +2953,13 @@
         <v>44</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2933,13 +2967,13 @@
         <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,13 +2981,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,13 +2995,13 @@
         <v>44</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2975,13 +3009,13 @@
         <v>44</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2989,13 +3023,13 @@
         <v>44</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3003,335 +3037,335 @@
         <v>44</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>459</v>
+      <c r="B32" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>628</v>
+        <v>466</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>629</v>
+      <c r="A46" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>475</v>
+        <v>628</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>477</v>
+      <c r="A50" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>479</v>
+        <v>629</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3339,13 +3373,13 @@
         <v>105</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3353,13 +3387,13 @@
         <v>105</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3367,811 +3401,811 @@
         <v>105</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>485</v>
+      <c r="A58" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>633</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>486</v>
+      <c r="A59" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>487</v>
+      <c r="A60" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>500</v>
+      <c r="A73" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>505</v>
+      <c r="A78" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>507</v>
+      <c r="A81" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>511</v>
+      <c r="A84" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>512</v>
+      <c r="A85" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>515</v>
+      <c r="A88" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>665</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>639</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B103" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C103" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D103" s="16" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="C97" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="B101" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="B102" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>655</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>651</v>
-      </c>
-    </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>631</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>652</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>653</v>
+      <c r="A104" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C104" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B105" s="13" t="s">
-        <v>632</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>656</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>654</v>
+      <c r="A105" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C105" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>657</v>
+        <v>667</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>685</v>
+        <v>692</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>657</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>634</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>659</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>686</v>
+      <c r="A107" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C107" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
-        <v>660</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>635</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>661</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>687</v>
+      <c r="A108" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C108" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>636</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>662</v>
-      </c>
-      <c r="D109" s="13" t="s">
-        <v>688</v>
+      <c r="A109" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>158</v>
+        <v>421</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B111" s="13" t="s">
-        <v>638</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>664</v>
-      </c>
-      <c r="D111" s="13" t="s">
-        <v>690</v>
+      <c r="A111" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
-        <v>665</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>639</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>666</v>
-      </c>
-      <c r="D112" s="13" t="s">
-        <v>691</v>
+      <c r="A112" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>667</v>
+        <v>421</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
+      <c r="A114" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="B114" s="13" t="s">
-        <v>641</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>669</v>
-      </c>
-      <c r="D114" s="13" t="s">
-        <v>693</v>
+      <c r="B114" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4179,55 +4213,55 @@
         <v>421</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>694</v>
+        <v>701</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>421</v>
+        <v>672</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4235,27 +4269,27 @@
         <v>676</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="s">
-        <v>676</v>
-      </c>
-      <c r="B120" s="13" t="s">
-        <v>647</v>
-      </c>
-      <c r="C120" s="13" t="s">
-        <v>678</v>
-      </c>
-      <c r="D120" s="13" t="s">
-        <v>702</v>
+      <c r="A120" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4300,20 +4334,52 @@
         <v>700</v>
       </c>
     </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="C124" s="18" t="s">
+        <v>705</v>
+      </c>
+      <c r="D124" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B125" s="18" t="s">
+        <v>706</v>
+      </c>
+      <c r="C125" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="D125" t="s">
+        <v>707</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D123"/>
+  <autoFilter ref="A1:D123" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D123">
+      <sortCondition ref="B1:B123"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,422 +4406,422 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>193</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>393</v>
+        <v>217</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>394</v>
+        <v>218</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>193</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>396</v>
+        <v>220</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>193</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>397</v>
+        <v>221</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>398</v>
+        <v>222</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>400</v>
+        <v>223</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>402</v>
+        <v>225</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>522</v>
+        <v>595</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>220</v>
+        <v>227</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>528</v>
+        <v>596</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>222</v>
+        <v>229</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>529</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>218</v>
+        <v>231</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>527</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>276</v>
+        <v>233</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>234</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>530</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>388</v>
+        <v>235</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>236</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>533</v>
+        <v>599</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>390</v>
+        <v>237</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>238</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>532</v>
+        <v>600</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>392</v>
+        <v>239</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>531</v>
+        <v>601</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>534</v>
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>535</v>
+        <v>244</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>536</v>
+        <v>246</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>537</v>
+        <v>248</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>538</v>
+        <v>250</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>539</v>
+        <v>252</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>540</v>
+        <v>254</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>541</v>
+        <v>256</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>542</v>
+        <v>258</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>543</v>
+        <v>259</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>544</v>
+        <v>261</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>545</v>
+        <v>264</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>546</v>
+        <v>266</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>547</v>
+        <v>268</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>548</v>
+        <v>270</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>549</v>
+        <v>272</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>550</v>
+        <v>274</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>551</v>
+        <v>275</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4763,13 +4829,13 @@
         <v>143</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>311</v>
+        <v>277</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>312</v>
+        <v>278</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,13 +4843,13 @@
         <v>143</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,13 +4857,13 @@
         <v>143</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,13 +4871,13 @@
         <v>143</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>318</v>
+        <v>284</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4819,13 +4885,13 @@
         <v>143</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>319</v>
+        <v>285</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4833,13 +4899,13 @@
         <v>143</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4847,13 +4913,13 @@
         <v>143</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4861,13 +4927,13 @@
         <v>143</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4875,13 +4941,13 @@
         <v>143</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>560</v>
+        <v>543</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4889,13 +4955,13 @@
         <v>143</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4903,13 +4969,13 @@
         <v>143</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>562</v>
+        <v>298</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4917,13 +4983,13 @@
         <v>143</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>563</v>
+        <v>546</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4931,13 +4997,13 @@
         <v>143</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>564</v>
+        <v>547</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4945,13 +5011,13 @@
         <v>143</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>565</v>
+        <v>548</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4959,13 +5025,13 @@
         <v>143</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>566</v>
+        <v>549</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4973,13 +5039,13 @@
         <v>143</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>567</v>
+        <v>550</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4987,13 +5053,13 @@
         <v>143</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>568</v>
+        <v>551</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,13 +5067,13 @@
         <v>143</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>345</v>
+        <v>311</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>569</v>
+        <v>552</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -5015,13 +5081,13 @@
         <v>143</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>570</v>
+        <v>553</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -5029,13 +5095,13 @@
         <v>143</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>571</v>
+        <v>554</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -5043,13 +5109,13 @@
         <v>143</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>352</v>
+        <v>318</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>572</v>
+        <v>555</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -5057,13 +5123,13 @@
         <v>143</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>353</v>
+        <v>319</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>573</v>
+        <v>556</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5071,13 +5137,13 @@
         <v>143</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>355</v>
+        <v>321</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>574</v>
+        <v>557</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5085,13 +5151,13 @@
         <v>143</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>357</v>
+        <v>323</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>358</v>
+        <v>324</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5099,13 +5165,13 @@
         <v>143</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>576</v>
+        <v>559</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5113,13 +5179,13 @@
         <v>143</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>361</v>
+        <v>327</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5127,13 +5193,13 @@
         <v>143</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>364</v>
+        <v>330</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5141,13 +5207,13 @@
         <v>143</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5155,13 +5221,13 @@
         <v>143</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5169,13 +5235,13 @@
         <v>143</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,13 +5249,13 @@
         <v>143</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>582</v>
+        <v>565</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,13 +5263,13 @@
         <v>143</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>583</v>
+        <v>566</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,13 +5277,13 @@
         <v>143</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>584</v>
+        <v>567</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,13 +5291,13 @@
         <v>143</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>378</v>
+        <v>344</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>585</v>
+        <v>568</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -5239,13 +5305,13 @@
         <v>143</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -5253,391 +5319,391 @@
         <v>143</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>233</v>
+        <v>349</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>588</v>
+        <v>350</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>263</v>
+        <v>351</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>590</v>
+        <v>352</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>589</v>
+        <v>354</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>267</v>
+        <v>355</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>591</v>
+        <v>356</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>269</v>
+        <v>357</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>592</v>
+        <v>358</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>271</v>
+        <v>359</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>593</v>
+        <v>360</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>273</v>
+        <v>361</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>594</v>
+        <v>362</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>225</v>
+        <v>363</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>595</v>
+        <v>364</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>227</v>
+        <v>365</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>596</v>
+        <v>366</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>229</v>
+        <v>367</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>597</v>
+        <v>368</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>231</v>
+        <v>369</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>598</v>
+        <v>370</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>235</v>
+        <v>371</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>599</v>
+        <v>372</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>600</v>
+        <v>374</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>239</v>
+        <v>375</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>601</v>
+        <v>376</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>241</v>
+        <v>377</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>602</v>
+        <v>378</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>243</v>
+        <v>379</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>603</v>
+        <v>380</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>245</v>
+        <v>381</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>604</v>
+        <v>382</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>247</v>
+        <v>383</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>248</v>
+        <v>384</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>605</v>
+        <v>623</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>249</v>
+        <v>385</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>250</v>
+        <v>386</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>606</v>
+        <v>624</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>252</v>
+        <v>387</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>388</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>607</v>
+        <v>533</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>254</v>
+        <v>389</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>390</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>608</v>
+        <v>532</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>256</v>
+        <v>391</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>392</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>609</v>
+        <v>531</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>258</v>
+        <v>393</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>394</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>610</v>
+        <v>526</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>259</v>
+        <v>395</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>260</v>
+        <v>396</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>611</v>
+        <v>525</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>261</v>
+        <v>397</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>262</v>
+        <v>398</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>612</v>
+        <v>524</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>400</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>613</v>
+        <v>523</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>406</v>
+        <v>401</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>402</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>614</v>
+        <v>522</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -5645,13 +5711,13 @@
         <v>196</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -5659,13 +5725,13 @@
         <v>196</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -5673,13 +5739,13 @@
         <v>196</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -5687,13 +5753,13 @@
         <v>196</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -5701,13 +5767,13 @@
         <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -5715,55 +5781,55 @@
         <v>196</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>383</v>
+        <v>417</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>384</v>
+        <v>418</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>385</v>
+        <v>419</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>386</v>
+        <v>420</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -5809,17 +5875,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D106"/>
+  <autoFilter ref="A1:D106" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D106">
+      <sortCondition ref="B1:B106"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -8618,28 +8688,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D199"/>
+  <autoFilter ref="A1:D199" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D199">
+      <sortCondition ref="B1:B199"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8753,10 +8812,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8777,17 +8859,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added new layouts (and new ourairports data)
</commit_message>
<xml_diff>
--- a/data/APT_BBOX.xlsx
+++ b/data/APT_BBOX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speeters\repos\airport-dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spi\dev\repos\airport-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFD804C-E902-49D6-8BCD-C25B50F39997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE650E6-B37F-4033-894D-39449B678D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7590" yWindow="540" windowWidth="19515" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">All!$A$1:$D$199</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$132</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NO Monit.'!$A$1:$D$106</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="728">
   <si>
     <t>AIRPORT</t>
   </si>
@@ -2159,13 +2159,81 @@
   </si>
   <si>
     <t>Varna</t>
+  </si>
+  <si>
+    <t>EHEH</t>
+  </si>
+  <si>
+    <t>Eindhoven</t>
+  </si>
+  <si>
+    <t>5.355492,51.434267,5.395060,51.466146</t>
+  </si>
+  <si>
+    <t>ENBO</t>
+  </si>
+  <si>
+    <r>
+      <t>Bod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Footlight MT Light"/>
+        <family val="1"/>
+      </rPr>
+      <t>ø</t>
+    </r>
+  </si>
+  <si>
+    <t>14.299650,67.252138,14.422131,67.277083</t>
+  </si>
+  <si>
+    <t>ENTC</t>
+  </si>
+  <si>
+    <t>Tromsø</t>
+  </si>
+  <si>
+    <t>18.893566,69.667587,18.934422,69.698699</t>
+  </si>
+  <si>
+    <t>18.440037,54.367258,18.504324,54.386256</t>
+  </si>
+  <si>
+    <t>LGRP</t>
+  </si>
+  <si>
+    <t>Rodos</t>
+  </si>
+  <si>
+    <t>28.062901,36.396622,28.110580,36.413616</t>
+  </si>
+  <si>
+    <t>Bari Karol Wojtyla</t>
+  </si>
+  <si>
+    <t>LIBD</t>
+  </si>
+  <si>
+    <t>LIEO</t>
+  </si>
+  <si>
+    <t>Olbia Costa Smeralda</t>
+  </si>
+  <si>
+    <t>9.500213,40.888828,9.537077,40.909783</t>
+  </si>
+  <si>
+    <t>16.729302,41.127308,16.778569,41.145796</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2187,6 +2255,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Footlight MT Light"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2215,12 +2289,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2269,12 +2343,139 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2307,15 +2508,32 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2597,11 +2815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,17 +2844,17 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="15" t="s">
         <v>429</v>
       </c>
     </row>
@@ -2654,31 +2872,31 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="16" t="s">
         <v>432</v>
       </c>
     </row>
@@ -2832,7 +3050,7 @@
       <c r="C16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>443</v>
       </c>
     </row>
@@ -2860,7 +3078,7 @@
       <c r="C18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="13" t="s">
         <v>431</v>
       </c>
     </row>
@@ -2878,59 +3096,59 @@
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="18" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="19" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="19" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="20" t="s">
         <v>655</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="20" t="s">
         <v>651</v>
       </c>
     </row>
@@ -3047,16 +3265,16 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>631</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="13" t="s">
         <v>652</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="13" t="s">
         <v>653</v>
       </c>
     </row>
@@ -3102,116 +3320,116 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="18" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="16" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>709</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>710</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="16" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B40" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="18" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B41" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C41" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="19" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="19" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>466</v>
+      <c r="B43" s="16" t="s">
+        <v>712</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,13 +3437,13 @@
         <v>82</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,363 +3451,363 @@
         <v>82</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>601</v>
+      <c r="A46" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B49" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C51" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D51" s="18" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B52" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C52" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D52" s="16" t="s">
         <v>628</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>632</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B57" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C57" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D57" s="16" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B61" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C61" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D61" s="18" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
         <v>657</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B62" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C62" s="20" t="s">
         <v>658</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D62" s="20" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="17" t="s">
         <v>657</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B63" s="17" t="s">
         <v>634</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>659</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D63" s="17" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
         <v>660</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B64" s="22" t="s">
         <v>635</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C64" s="22" t="s">
         <v>661</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D64" s="22" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B65" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C65" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D65" s="37" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>704</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>705</v>
+      </c>
+      <c r="D66" s="36" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>706</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>708</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B68" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C68" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D68" s="19" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B69" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C69" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D69" s="19" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B70" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C70" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D70" s="16" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,13 +3815,13 @@
         <v>105</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,111 +3829,111 @@
         <v>105</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>537</v>
+      <c r="A73" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>571</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>495</v>
+      <c r="A79" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3723,27 +3941,27 @@
         <v>143</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>582</v>
+      <c r="A81" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3751,621 +3969,719 @@
         <v>143</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>662</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>688</v>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>637</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>663</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>689</v>
+      <c r="A85" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>636</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>719</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>720</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B93" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C93" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D93" s="19" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B94" s="16" t="s">
+        <v>723</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C95" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D95" s="23" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B96" s="13" t="s">
         <v>638</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C96" s="13" t="s">
         <v>664</v>
       </c>
-      <c r="D88" s="17" t="s">
+      <c r="D96" s="13" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B97" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D98" s="6" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B99" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="D99" s="6" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B100" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C100" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D100" s="6" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B101" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C101" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="D101" s="6" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B102" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D102" s="6" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B103" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D103" s="6" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B95" s="16" t="s">
+      <c r="B104" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C95" s="16" t="s">
+      <c r="C104" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="D95" s="16" t="s">
+      <c r="D104" s="12" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B105" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C105" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D96" s="16" t="s">
+      <c r="D105" s="12" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B106" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C97" s="16" t="s">
+      <c r="C106" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D106" s="25" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
+    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B107" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="C98" s="16" t="s">
+      <c r="C107" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="D98" s="16" t="s">
+      <c r="D107" s="26" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B108" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C99" s="16" t="s">
+      <c r="C108" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="D99" s="16" t="s">
+      <c r="D108" s="26" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="28" t="s">
         <v>665</v>
       </c>
-      <c r="B100" s="13" t="s">
+      <c r="B109" s="28" t="s">
         <v>639</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C109" s="28" t="s">
         <v>666</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D109" s="28" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="B101" s="16" t="s">
+      <c r="B110" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C101" s="16" t="s">
+      <c r="C110" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D101" s="16" t="s">
+      <c r="D110" s="26" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="B111" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C102" s="16" t="s">
+      <c r="C111" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D102" s="16" t="s">
+      <c r="D111" s="26" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
+    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B112" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C103" s="16" t="s">
+      <c r="C112" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="D103" s="16" t="s">
+      <c r="D112" s="26" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="B104" s="16" t="s">
+      <c r="B113" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="C104" s="16" t="s">
+      <c r="C113" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="D113" s="24" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B105" s="16" t="s">
+      <c r="B114" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C105" s="16" t="s">
+      <c r="C114" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D105" s="16" t="s">
+      <c r="D114" s="12" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
+    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="29" t="s">
         <v>667</v>
       </c>
-      <c r="B106" s="13" t="s">
+      <c r="B115" s="29" t="s">
         <v>640</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C115" s="29" t="s">
         <v>668</v>
       </c>
-      <c r="D106" s="13" t="s">
+      <c r="D115" s="29" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="B107" s="16" t="s">
+      <c r="B116" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="C107" s="16" t="s">
+      <c r="C116" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="D107" s="16" t="s">
+      <c r="D116" s="26" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="B108" s="16" t="s">
+      <c r="B117" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="C108" s="16" t="s">
+      <c r="C117" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="D108" s="16" t="s">
+      <c r="D117" s="30" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B109" s="16" t="s">
+      <c r="B118" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="C118" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="D109" s="16" t="s">
+      <c r="D118" s="31" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="27" t="s">
         <v>421</v>
       </c>
-      <c r="B110" s="13" t="s">
+      <c r="B119" s="27" t="s">
         <v>641</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C119" s="27" t="s">
         <v>669</v>
       </c>
-      <c r="D110" s="13" t="s">
+      <c r="D119" s="27" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B120" s="32" t="s">
         <v>422</v>
       </c>
-      <c r="C111" s="14" t="s">
+      <c r="C120" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="D111" s="14" t="s">
+      <c r="D120" s="32" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B121" s="32" t="s">
         <v>424</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C121" s="32" t="s">
         <v>425</v>
       </c>
-      <c r="D112" s="14" t="s">
+      <c r="D121" s="32" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="B113" s="13" t="s">
+      <c r="B122" s="32" t="s">
         <v>642</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C122" s="32" t="s">
         <v>670</v>
       </c>
-      <c r="D113" s="13" t="s">
+      <c r="D122" s="32" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="14" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B123" s="32" t="s">
         <v>426</v>
       </c>
-      <c r="C114" s="14" t="s">
+      <c r="C123" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="D114" s="14" t="s">
+      <c r="D123" s="32" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="s">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="B115" s="13" t="s">
+      <c r="B124" s="33" t="s">
         <v>643</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C124" s="33" t="s">
         <v>671</v>
       </c>
-      <c r="D115" s="13" t="s">
+      <c r="D124" s="33" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="28" t="s">
         <v>672</v>
       </c>
-      <c r="B116" s="13" t="s">
+      <c r="B125" s="28" t="s">
         <v>644</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C125" s="28" t="s">
         <v>673</v>
       </c>
-      <c r="D116" s="13" t="s">
+      <c r="D125" s="28" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="s">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="28" t="s">
         <v>674</v>
       </c>
-      <c r="B117" s="13" t="s">
+      <c r="B126" s="28" t="s">
         <v>645</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C126" s="28" t="s">
         <v>675</v>
       </c>
-      <c r="D117" s="13" t="s">
+      <c r="D126" s="28" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="13" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="27" t="s">
         <v>676</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B127" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C127" s="27" t="s">
         <v>677</v>
       </c>
-      <c r="D118" s="13" t="s">
+      <c r="D127" s="27" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
+    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="B119" s="13" t="s">
+      <c r="B128" s="33" t="s">
         <v>647</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="C128" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="D119" s="13" t="s">
+      <c r="D128" s="33" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B129" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="C129" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D120" s="16" t="s">
+      <c r="D129" s="26" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="28" t="s">
         <v>679</v>
       </c>
-      <c r="B121" s="13" t="s">
+      <c r="B130" s="28" t="s">
         <v>648</v>
       </c>
-      <c r="C121" s="13" t="s">
+      <c r="C130" s="28" t="s">
         <v>680</v>
       </c>
-      <c r="D121" s="13" t="s">
+      <c r="D130" s="28" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="28" t="s">
         <v>681</v>
       </c>
-      <c r="B122" s="13" t="s">
+      <c r="B131" s="28" t="s">
         <v>649</v>
       </c>
-      <c r="C122" s="13" t="s">
+      <c r="C131" s="28" t="s">
         <v>682</v>
       </c>
-      <c r="D122" s="13" t="s">
+      <c r="D131" s="28" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="s">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="28" t="s">
         <v>683</v>
       </c>
-      <c r="B123" s="13" t="s">
+      <c r="B132" s="28" t="s">
         <v>650</v>
       </c>
-      <c r="C123" s="13" t="s">
+      <c r="C132" s="28" t="s">
         <v>684</v>
       </c>
-      <c r="D123" s="13" t="s">
+      <c r="D132" s="28" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B124" s="18" t="s">
-        <v>704</v>
-      </c>
-      <c r="C124" s="18" t="s">
-        <v>705</v>
-      </c>
-      <c r="D124" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B125" s="18" t="s">
-        <v>706</v>
-      </c>
-      <c r="C125" s="18" t="s">
-        <v>708</v>
-      </c>
-      <c r="D125" t="s">
-        <v>707</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D123" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D123">
-      <sortCondition ref="B1:B123"/>
+  <autoFilter ref="A1:D132" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D132">
+      <sortCondition ref="B1:B132"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5953,7 +6269,7 @@
       <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>430</v>
       </c>
     </row>
@@ -8699,6 +9015,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -8812,33 +9143,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8859,9 +9167,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
BIKF bounding box added to APT_BBOX.xlsx
</commit_message>
<xml_diff>
--- a/data/APT_BBOX.xlsx
+++ b/data/APT_BBOX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spi\dev\repos\airport-dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speeters\repos\airport-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE650E6-B37F-4033-894D-39449B678D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AE4EA-7EB8-48CB-A5DF-B838B4937276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7590" yWindow="540" windowWidth="19515" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="6" r:id="rId1"/>
@@ -19,20 +19,31 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">All!$A$1:$D$199</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$133</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NO Monit.'!$A$1:$D$106</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="732">
   <si>
     <t>AIRPORT</t>
   </si>
@@ -2227,6 +2238,18 @@
   </si>
   <si>
     <t>16.729302,41.127308,16.778569,41.145796</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>BIKF</t>
+  </si>
+  <si>
+    <t>Keflavik</t>
+  </si>
+  <si>
+    <t>-22.64,63.98,-22.56,64.02</t>
   </si>
 </sst>
 </file>
@@ -2475,7 +2498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2511,7 +2534,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2526,7 +2548,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2534,6 +2556,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2815,11 +2839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,74 +2868,74 @@
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>728</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>729</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="6" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,13 +2943,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>434</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2933,13 +2957,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,13 +2971,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,13 +2985,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2975,13 +2999,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2989,13 +3013,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3003,13 +3027,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3017,13 +3041,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3031,13 +3055,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3045,13 +3069,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>443</v>
+        <v>26</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3059,13 +3083,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>442</v>
+        <v>28</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3073,13 +3097,13 @@
         <v>7</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>431</v>
+        <v>30</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,83 +3111,83 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D21" s="17" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>630</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>655</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D24" s="19" t="s">
         <v>651</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3171,13 +3195,13 @@
         <v>44</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3185,13 +3209,13 @@
         <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3199,13 +3223,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3213,13 +3237,13 @@
         <v>44</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,13 +3251,13 @@
         <v>44</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3241,13 +3265,13 @@
         <v>44</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,41 +3279,41 @@
         <v>44</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>631</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C33" s="13" t="s">
         <v>652</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>653</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3297,13 +3321,13 @@
         <v>44</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3311,139 +3335,139 @@
         <v>44</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C37" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D37" s="17" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D38" s="15" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B39" s="17" t="s">
         <v>709</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>710</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D39" s="17" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C40" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D40" s="15" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C42" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D42" s="18" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C43" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D43" s="18" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>712</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>713</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3451,13 +3475,13 @@
         <v>82</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,13 +3489,13 @@
         <v>82</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>715</v>
+        <v>84</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>716</v>
+        <v>85</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>717</v>
+        <v>466</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3479,167 +3503,167 @@
         <v>82</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B49" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C49" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D49" s="17" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B50" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C50" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D50" s="20" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+    <row r="51" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B52" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C52" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D52" s="17" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B53" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C53" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D53" s="15" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C55" s="16" t="s">
         <v>656</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D55" s="16" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="19" t="s">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C56" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D56" s="18" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="19" t="s">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B57" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C57" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D57" s="18" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B58" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D58" s="15" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3647,13 +3671,13 @@
         <v>105</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3661,167 +3685,167 @@
         <v>105</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B62" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C62" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D62" s="17" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>657</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>633</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C63" s="19" t="s">
         <v>658</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D63" s="19" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="17" t="s">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
         <v>657</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>634</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C64" s="16" t="s">
         <v>659</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D64" s="16" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="22" t="s">
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="21" t="s">
         <v>660</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B65" s="21" t="s">
         <v>635</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C65" s="21" t="s">
         <v>661</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D65" s="21" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="37" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="37" t="s">
+      <c r="B66" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="C66" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D66" s="36" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B66" s="35" t="s">
-        <v>704</v>
-      </c>
-      <c r="C66" s="35" t="s">
-        <v>705</v>
-      </c>
-      <c r="D66" s="36" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="s">
         <v>116</v>
       </c>
       <c r="B67" s="34" t="s">
+        <v>704</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>705</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="33" t="s">
         <v>706</v>
       </c>
-      <c r="C67" s="34" t="s">
+      <c r="C68" s="33" t="s">
         <v>708</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D68" s="14" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B69" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C69" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D69" s="18" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="19" t="s">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="B70" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C70" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D70" s="18" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B71" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C71" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D71" s="15" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3829,13 +3853,13 @@
         <v>105</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3843,13 +3867,13 @@
         <v>105</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,13 +3881,13 @@
         <v>105</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3871,13 +3895,13 @@
         <v>105</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3885,13 +3909,13 @@
         <v>105</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3899,55 +3923,55 @@
         <v>105</v>
       </c>
       <c r="B77" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D78" s="6" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="18" t="s">
+    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B79" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C79" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D79" s="17" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B79" s="21" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="C80" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="D79" s="21" t="s">
+      <c r="D80" s="20" t="s">
         <v>537</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,13 +3979,13 @@
         <v>143</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3969,13 +3993,13 @@
         <v>143</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3983,41 +4007,41 @@
         <v>143</v>
       </c>
       <c r="B83" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D84" s="6" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B84" s="13" t="s">
+    <row r="85" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C85" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="13" t="s">
         <v>571</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4025,69 +4049,69 @@
         <v>143</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D87" s="6" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B87" s="13" t="s">
+    <row r="88" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C88" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D88" s="13" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B88" s="18" t="s">
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B89" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C89" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="D88" s="18" t="s">
+      <c r="D89" s="17" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B90" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="C89" s="16" t="s">
+      <c r="C90" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D90" s="15" t="s">
         <v>498</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>636</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>662</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4095,97 +4119,97 @@
         <v>158</v>
       </c>
       <c r="B91" s="13" t="s">
+        <v>636</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="13" t="s">
         <v>719</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C92" s="13" t="s">
         <v>720</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D92" s="13" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="17" t="s">
+    <row r="93" spans="1:4" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B93" s="16" t="s">
         <v>637</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C93" s="16" t="s">
         <v>663</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D93" s="16" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="19" t="s">
+    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B94" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C94" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D94" s="18" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B95" s="15" t="s">
         <v>723</v>
       </c>
-      <c r="C94" s="16" t="s">
+      <c r="C95" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="D95" s="15" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="23" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="B95" s="23" t="s">
+      <c r="B96" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C96" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D95" s="23" t="s">
+      <c r="D96" s="22" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B97" s="13" t="s">
         <v>638</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C97" s="13" t="s">
         <v>664</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D97" s="13" t="s">
         <v>690</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>724</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4193,13 +4217,13 @@
         <v>164</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>166</v>
+        <v>724</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>167</v>
+        <v>725</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>502</v>
+        <v>726</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4207,13 +4231,13 @@
         <v>164</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4221,13 +4245,13 @@
         <v>164</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4235,13 +4259,13 @@
         <v>164</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,13 +4273,13 @@
         <v>164</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4263,27 +4287,27 @@
         <v>164</v>
       </c>
       <c r="B103" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C104" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="D104" s="6" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4291,397 +4315,411 @@
         <v>164</v>
       </c>
       <c r="B105" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B106" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C106" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D105" s="12" t="s">
+      <c r="D106" s="12" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="25" t="s">
+    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B106" s="25" t="s">
+      <c r="B107" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="C106" s="25" t="s">
+      <c r="C107" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="D106" s="25" t="s">
+      <c r="D107" s="24" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="26" t="s">
+    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B108" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C107" s="26" t="s">
+      <c r="C108" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="D107" s="26" t="s">
+      <c r="D108" s="25" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="26" t="s">
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="B108" s="26" t="s">
+      <c r="B109" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="26" t="s">
+      <c r="C109" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="D108" s="26" t="s">
+      <c r="D109" s="25" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="28" t="s">
+    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="27" t="s">
         <v>665</v>
       </c>
-      <c r="B109" s="28" t="s">
+      <c r="B110" s="27" t="s">
         <v>639</v>
       </c>
-      <c r="C109" s="28" t="s">
+      <c r="C110" s="27" t="s">
         <v>666</v>
       </c>
-      <c r="D109" s="28" t="s">
+      <c r="D110" s="27" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="26" t="s">
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="B110" s="26" t="s">
+      <c r="B111" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C110" s="26" t="s">
+      <c r="C111" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="D110" s="26" t="s">
+      <c r="D111" s="25" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="26" t="s">
+    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B112" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="C111" s="26" t="s">
+      <c r="C112" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D111" s="26" t="s">
+      <c r="D112" s="25" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="26" t="s">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B112" s="26" t="s">
+      <c r="B113" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C112" s="26" t="s">
+      <c r="C113" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="D112" s="26" t="s">
+      <c r="D113" s="25" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="24" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B113" s="24" t="s">
+      <c r="B114" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="C113" s="24" t="s">
+      <c r="C114" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="D113" s="24" t="s">
+      <c r="D114" s="23" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B115" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C115" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D115" s="12" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="29" t="s">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="28" t="s">
         <v>667</v>
       </c>
-      <c r="B115" s="29" t="s">
+      <c r="B116" s="28" t="s">
         <v>640</v>
       </c>
-      <c r="C115" s="29" t="s">
+      <c r="C116" s="28" t="s">
         <v>668</v>
       </c>
-      <c r="D115" s="29" t="s">
+      <c r="D116" s="28" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="26" t="s">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B117" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="C117" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="D116" s="26" t="s">
+      <c r="D117" s="25" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="30" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="B117" s="30" t="s">
+      <c r="B118" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="C117" s="30" t="s">
+      <c r="C118" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="D117" s="30" t="s">
+      <c r="D118" s="29" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="31" t="s">
+    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="B118" s="31" t="s">
+      <c r="B119" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="C118" s="31" t="s">
+      <c r="C119" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="D118" s="31" t="s">
+      <c r="D119" s="30" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="27" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="B119" s="27" t="s">
+      <c r="B120" s="26" t="s">
         <v>641</v>
       </c>
-      <c r="C119" s="27" t="s">
+      <c r="C120" s="26" t="s">
         <v>669</v>
       </c>
-      <c r="D119" s="27" t="s">
+      <c r="D120" s="26" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="32" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="B120" s="32" t="s">
+      <c r="B121" s="31" t="s">
         <v>422</v>
       </c>
-      <c r="C120" s="32" t="s">
+      <c r="C121" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="D120" s="32" t="s">
+      <c r="D121" s="31" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="32" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="B121" s="32" t="s">
+      <c r="B122" s="31" t="s">
         <v>424</v>
       </c>
-      <c r="C121" s="32" t="s">
+      <c r="C122" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="D121" s="32" t="s">
+      <c r="D122" s="31" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="32" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="B122" s="32" t="s">
+      <c r="B123" s="31" t="s">
         <v>642</v>
       </c>
-      <c r="C122" s="32" t="s">
+      <c r="C123" s="31" t="s">
         <v>670</v>
       </c>
-      <c r="D122" s="32" t="s">
+      <c r="D123" s="31" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="32" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="B123" s="32" t="s">
+      <c r="B124" s="31" t="s">
         <v>426</v>
       </c>
-      <c r="C123" s="32" t="s">
+      <c r="C124" s="31" t="s">
         <v>427</v>
       </c>
-      <c r="D123" s="32" t="s">
+      <c r="D124" s="31" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="33" t="s">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="32" t="s">
         <v>421</v>
       </c>
-      <c r="B124" s="33" t="s">
+      <c r="B125" s="32" t="s">
         <v>643</v>
       </c>
-      <c r="C124" s="33" t="s">
+      <c r="C125" s="32" t="s">
         <v>671</v>
       </c>
-      <c r="D124" s="33" t="s">
+      <c r="D125" s="32" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="28" t="s">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="27" t="s">
         <v>672</v>
       </c>
-      <c r="B125" s="28" t="s">
+      <c r="B126" s="27" t="s">
         <v>644</v>
       </c>
-      <c r="C125" s="28" t="s">
+      <c r="C126" s="27" t="s">
         <v>673</v>
       </c>
-      <c r="D125" s="28" t="s">
+      <c r="D126" s="27" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="28" t="s">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="27" t="s">
         <v>674</v>
       </c>
-      <c r="B126" s="28" t="s">
+      <c r="B127" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="C126" s="28" t="s">
+      <c r="C127" s="27" t="s">
         <v>675</v>
       </c>
-      <c r="D126" s="28" t="s">
+      <c r="D127" s="27" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="27" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="26" t="s">
         <v>676</v>
       </c>
-      <c r="B127" s="27" t="s">
+      <c r="B128" s="26" t="s">
         <v>646</v>
       </c>
-      <c r="C127" s="27" t="s">
+      <c r="C128" s="26" t="s">
         <v>677</v>
       </c>
-      <c r="D127" s="27" t="s">
+      <c r="D128" s="26" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="33" t="s">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="32" t="s">
         <v>676</v>
       </c>
-      <c r="B128" s="33" t="s">
+      <c r="B129" s="32" t="s">
         <v>647</v>
       </c>
-      <c r="C128" s="33" t="s">
+      <c r="C129" s="32" t="s">
         <v>678</v>
       </c>
-      <c r="D128" s="33" t="s">
+      <c r="D129" s="32" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="26" t="s">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="B129" s="26" t="s">
+      <c r="B130" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="C129" s="26" t="s">
+      <c r="C130" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D129" s="26" t="s">
+      <c r="D130" s="25" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="28" t="s">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="27" t="s">
         <v>679</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="B131" s="27" t="s">
         <v>648</v>
       </c>
-      <c r="C130" s="28" t="s">
+      <c r="C131" s="27" t="s">
         <v>680</v>
       </c>
-      <c r="D130" s="28" t="s">
+      <c r="D131" s="27" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="28" t="s">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="27" t="s">
         <v>681</v>
       </c>
-      <c r="B131" s="28" t="s">
+      <c r="B132" s="27" t="s">
         <v>649</v>
       </c>
-      <c r="C131" s="28" t="s">
+      <c r="C132" s="27" t="s">
         <v>682</v>
       </c>
-      <c r="D131" s="28" t="s">
+      <c r="D132" s="27" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="28" t="s">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="27" t="s">
         <v>683</v>
       </c>
-      <c r="B132" s="28" t="s">
+      <c r="B133" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C132" s="28" t="s">
+      <c r="C133" s="27" t="s">
         <v>684</v>
       </c>
-      <c r="D132" s="28" t="s">
+      <c r="D133" s="27" t="s">
         <v>700</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D132" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D132">
-      <sortCondition ref="B1:B132"/>
+  <autoFilter ref="A1:D133" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D133">
+      <sortCondition ref="B1:B133"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4694,7 +4732,7 @@
   <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
@@ -6205,7 +6243,7 @@
   <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -9015,21 +9053,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -9143,10 +9166,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9167,17 +9213,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
BIKF bounding box updated to show runways correctly
</commit_message>
<xml_diff>
--- a/data/APT_BBOX.xlsx
+++ b/data/APT_BBOX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speeters\repos\airport-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AE4EA-7EB8-48CB-A5DF-B838B4937276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61A2BD4-1882-43E2-BAC2-4B754901DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="6" r:id="rId1"/>
@@ -2249,7 +2249,7 @@
     <t>Keflavik</t>
   </si>
   <si>
-    <t>-22.64,63.98,-22.56,64.02</t>
+    <t>-22.66,63.95,-22.56,64.02</t>
   </si>
 </sst>
 </file>
@@ -2843,7 +2843,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9053,6 +9053,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -9166,33 +9181,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9213,9 +9205,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UGKO and UGSB added
</commit_message>
<xml_diff>
--- a/data/APT_BBOX.xlsx
+++ b/data/APT_BBOX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speeters\repos\airport-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61A2BD4-1882-43E2-BAC2-4B754901DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E635CD5-8C93-4875-84E2-2D11E72B4E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitored" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">All!$A$1:$D$199</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitored!$A$1:$D$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NO Monit.'!$A$1:$D$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="738">
   <si>
     <t>AIRPORT</t>
   </si>
@@ -2250,6 +2250,24 @@
   </si>
   <si>
     <t>-22.66,63.95,-22.56,64.02</t>
+  </si>
+  <si>
+    <t>UGKO</t>
+  </si>
+  <si>
+    <t>UGSB</t>
+  </si>
+  <si>
+    <t>KUTAISI/KOPITNARI</t>
+  </si>
+  <si>
+    <t>BATUMI</t>
+  </si>
+  <si>
+    <t>42.449155932401624, 42.16127844861186, 42.51086819741627, 42.193085785014325</t>
+  </si>
+  <si>
+    <t>41.58398308014017, 41.598667543454965, 41.615869180909215, 41.62003973073927</t>
   </si>
 </sst>
 </file>
@@ -2498,7 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2558,6 +2576,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2839,11 +2858,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4688,38 +4707,66 @@
         <v>698</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="27" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="39" t="s">
         <v>681</v>
       </c>
-      <c r="B132" s="27" t="s">
+      <c r="B132" s="39" t="s">
         <v>649</v>
       </c>
-      <c r="C132" s="27" t="s">
+      <c r="C132" s="39" t="s">
         <v>682</v>
       </c>
-      <c r="D132" s="27" t="s">
+      <c r="D132" s="39" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="27" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="39" t="s">
+        <v>681</v>
+      </c>
+      <c r="B133" s="31" t="s">
+        <v>732</v>
+      </c>
+      <c r="C133" t="s">
+        <v>734</v>
+      </c>
+      <c r="D133" s="31" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="39" t="s">
+        <v>681</v>
+      </c>
+      <c r="B134" s="31" t="s">
+        <v>733</v>
+      </c>
+      <c r="C134" t="s">
+        <v>735</v>
+      </c>
+      <c r="D134" s="31" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="27" t="s">
         <v>683</v>
       </c>
-      <c r="B133" s="27" t="s">
+      <c r="B135" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="C133" s="27" t="s">
+      <c r="C135" s="27" t="s">
         <v>684</v>
       </c>
-      <c r="D133" s="27" t="s">
+      <c r="D135" s="27" t="s">
         <v>700</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D133" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D133">
-      <sortCondition ref="B1:B133"/>
+  <autoFilter ref="A1:D135" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D135">
+      <sortCondition ref="B1:B135"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9053,21 +9100,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D0FE5D67A8955468C14E1CD507D7C7A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2136fc4bded2217ef16a7f65bc2a169">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -9181,10 +9213,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9205,17 +9260,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59517FD-2FEA-4C30-82FF-FAEC56890ACA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A91219-5C2C-423A-833B-AB294380AD1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fd60f3b8-f236-4830-aecc-da0a7fc54679}" enabled="1" method="Standard" siteId="{76f33c20-5979-4408-adf7-8b3c4be95e52}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>